<commit_message>
Added "Getting the Most Rare Resources by Tiles Available" in readme
</commit_message>
<xml_diff>
--- a/ReadMe Support/Tables in ReadMe.xlsx
+++ b/ReadMe Support/Tables in ReadMe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethhsu/Google Drive/Hsu Family/Kenneth Hsu/Projects/Colonizer/Github/ReadMe Support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8D687C-408C-5148-8149-6C70891BCA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00A4E4A-F5AD-724F-8FDF-4CBFC1C7B953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30120" yWindow="2700" windowWidth="28040" windowHeight="17440" xr2:uid="{6F4063CB-0874-6C41-89AE-ED10A26CD472}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>